<commit_message>
Updated version of data template
</commit_message>
<xml_diff>
--- a/www/data-entry-template/ATLAS_data_entry_template_v12.xlsx
+++ b/www/data-entry-template/ATLAS_data_entry_template_v12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benhlina/Library/CloudStorage/Dropbox/GitHub/NAAEDApp/www/data-entry-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3525A5F0-C0A2-AA49-AD92-96046C44097C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901536D6-FBE3-524F-BF14-B6A72B6BBA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19460" xr2:uid="{DE6F8925-643B-304C-8933-23D4A9123DA3}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19460" activeTab="2" xr2:uid="{DE6F8925-643B-304C-8933-23D4A9123DA3}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
@@ -205,9 +205,6 @@
     <t>common_name</t>
   </si>
   <si>
-    <t>scientific_name</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
@@ -988,6 +985,9 @@
   </si>
   <si>
     <t>tbl_length</t>
+  </si>
+  <si>
+    <t>genus_species</t>
   </si>
 </sst>
 </file>
@@ -1681,9 +1681,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+    <sheetView zoomScale="136" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1697,7 +1697,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="48" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="2" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B2" s="48"/>
       <c r="C2" s="48"/>
@@ -1727,940 +1727,940 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" s="45" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>114</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>117</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>119</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>121</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C19" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>123</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>126</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B23" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B24" s="39" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B25" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B27" s="39" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>7</v>
+        <v>231</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B31" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B32" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B35" s="40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B44" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C45" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B46" s="39" t="s">
-        <v>21</v>
-      </c>
       <c r="C46" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="56" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="56" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B52" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B53" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B57" s="44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B60" s="44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B61" s="44" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B63" s="39" t="s">
-        <v>35</v>
-      </c>
       <c r="C63" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B71" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="D71" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2696,17 +2696,17 @@
   <sheetData>
     <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -2717,57 +2717,57 @@
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
       <c r="D3" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="E4" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="F4" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="G4" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="H4" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="J4" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="K4" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="L4" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="J4" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="K4" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="L4" s="33" t="s">
+      <c r="M4" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="N4" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="N4" s="33" t="s">
+      <c r="O4" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="O4" s="33" t="s">
+      <c r="P4" s="33" t="s">
         <v>103</v>
-      </c>
-      <c r="P4" s="33" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2790,11 +2790,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AZ5"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="9" ySplit="5" topLeftCell="J6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2829,17 +2829,17 @@
   <sheetData>
     <row r="1" spans="1:52" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -2850,182 +2850,182 @@
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
       <c r="D3" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Z4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AG4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AQ4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AW4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:52" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="J5" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="24" t="s">
+      <c r="K5" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="S5" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="T5" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="U5" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="V5" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="W5" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="X5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y5" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z5" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA5" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC5" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD5" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE5" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="M5" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="N5" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="O5" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="P5" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q5" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="R5" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="S5" s="24" t="s">
+      <c r="AF5" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG5" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH5" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="AI5" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="AJ5" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="T5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="U5" s="24" t="s">
+      <c r="AK5" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="AL5" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="V5" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="W5" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="X5" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y5" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z5" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="AA5" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB5" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC5" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD5" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE5" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF5" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG5" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH5" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="AI5" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="AJ5" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="AK5" s="24" t="s">
+      <c r="AM5" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="AN5" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="AO5" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="AL5" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AM5" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="AN5" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="AO5" s="25" t="s">
+      <c r="AP5" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="AP5" s="25" t="s">
+      <c r="AQ5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR5" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="AS5" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="AT5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU5" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="AV5" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="AW5" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="AX5" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AY5" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="AZ5" s="24" t="s">
         <v>181</v>
-      </c>
-      <c r="AQ5" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="AR5" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="AS5" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT5" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="AU5" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV5" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AW5" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="AX5" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="AY5" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AZ5" s="24" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>